<commit_message>
added some cropped versions of images to try particle analysis with
</commit_message>
<xml_diff>
--- a/data/survival/Westcott/B_survival_12172024.xlsx
+++ b/data/survival/Westcott/B_survival_12172024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceleuchtenberger/Library/Mobile Documents/com~apple~CloudDocs/Documents/project-gigas-conditioning-GL/data/survival/Westcott/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AA385D4-340A-EB40-970A-4584A43A6956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69B1137-FA7C-ED49-B5F0-5755107244D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13280" yWindow="780" windowWidth="28040" windowHeight="17440" xr2:uid="{CA941532-24D2-184F-8B30-D5633C401736}"/>
+    <workbookView xWindow="3120" yWindow="1180" windowWidth="28040" windowHeight="17440" xr2:uid="{CA941532-24D2-184F-8B30-D5633C401736}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="40">
   <si>
     <t>bag_num</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Counted 46 in photo</t>
+  </si>
+  <si>
+    <t>bag_tag_num</t>
   </si>
 </sst>
 </file>
@@ -529,18 +532,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECCF0E53-B26D-5F4D-A696-5BB849B2395F}">
-  <dimension ref="A1:K131"/>
+  <dimension ref="A1:L131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="I126" sqref="I126:I131"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L116" sqref="L116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -566,16 +569,19 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -601,13 +607,16 @@
         <v>1</v>
       </c>
       <c r="I2">
+        <v>53</v>
+      </c>
+      <c r="J2">
         <v>51</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -633,13 +642,16 @@
         <v>2</v>
       </c>
       <c r="I3">
+        <v>78</v>
+      </c>
+      <c r="J3">
         <v>50</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -665,16 +677,19 @@
         <v>3</v>
       </c>
       <c r="I4">
+        <v>59</v>
+      </c>
+      <c r="J4">
         <v>49</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -700,16 +715,19 @@
         <v>4</v>
       </c>
       <c r="I5">
+        <v>36</v>
+      </c>
+      <c r="J5">
         <v>49</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -735,13 +753,16 @@
         <v>5</v>
       </c>
       <c r="I6">
+        <v>73</v>
+      </c>
+      <c r="J6">
         <v>45</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -767,13 +788,16 @@
         <v>6</v>
       </c>
       <c r="I7">
+        <v>67</v>
+      </c>
+      <c r="J7">
         <v>47</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -799,13 +823,16 @@
         <v>7</v>
       </c>
       <c r="I8">
+        <v>77</v>
+      </c>
+      <c r="J8">
         <v>49</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -831,16 +858,19 @@
         <v>8</v>
       </c>
       <c r="I9">
+        <v>62</v>
+      </c>
+      <c r="J9">
         <v>49</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -866,16 +896,19 @@
         <v>9</v>
       </c>
       <c r="I10">
+        <v>95</v>
+      </c>
+      <c r="J10">
         <v>45</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -901,16 +934,19 @@
         <v>10</v>
       </c>
       <c r="I11">
+        <v>72</v>
+      </c>
+      <c r="J11">
         <v>46</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -936,13 +972,16 @@
         <v>1</v>
       </c>
       <c r="I12">
+        <v>53</v>
+      </c>
+      <c r="J12">
         <v>51</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -968,16 +1007,19 @@
         <v>2</v>
       </c>
       <c r="I13">
+        <v>78</v>
+      </c>
+      <c r="J13">
         <v>48</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1003,13 +1045,16 @@
         <v>3</v>
       </c>
       <c r="I14">
+        <v>59</v>
+      </c>
+      <c r="J14">
         <v>50</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1035,16 +1080,19 @@
         <v>4</v>
       </c>
       <c r="I15">
+        <v>36</v>
+      </c>
+      <c r="J15">
         <v>51</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1070,16 +1118,19 @@
         <v>5</v>
       </c>
       <c r="I16">
+        <v>73</v>
+      </c>
+      <c r="J16">
         <v>45</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1105,16 +1156,19 @@
         <v>6</v>
       </c>
       <c r="I17">
+        <v>67</v>
+      </c>
+      <c r="J17">
         <v>47</v>
       </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1140,16 +1194,19 @@
         <v>7</v>
       </c>
       <c r="I18">
+        <v>77</v>
+      </c>
+      <c r="J18">
         <v>51</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1175,13 +1232,16 @@
         <v>8</v>
       </c>
       <c r="I19">
+        <v>62</v>
+      </c>
+      <c r="J19">
         <v>50</v>
       </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1207,16 +1267,19 @@
         <v>9</v>
       </c>
       <c r="I20">
+        <v>95</v>
+      </c>
+      <c r="J20">
         <v>48</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20" t="s">
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1242,13 +1305,16 @@
         <v>10</v>
       </c>
       <c r="I21">
+        <v>72</v>
+      </c>
+      <c r="J21">
         <v>46</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1274,13 +1340,16 @@
         <v>1</v>
       </c>
       <c r="I22">
+        <v>53</v>
+      </c>
+      <c r="J22">
         <v>50</v>
       </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1306,13 +1375,16 @@
         <v>2</v>
       </c>
       <c r="I23">
+        <v>78</v>
+      </c>
+      <c r="J23">
         <v>49</v>
       </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1338,13 +1410,16 @@
         <v>3</v>
       </c>
       <c r="I24">
+        <v>59</v>
+      </c>
+      <c r="J24">
         <v>50</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1370,13 +1445,16 @@
         <v>4</v>
       </c>
       <c r="I25">
+        <v>36</v>
+      </c>
+      <c r="J25">
         <v>50</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1402,13 +1480,16 @@
         <v>5</v>
       </c>
       <c r="I26">
+        <v>73</v>
+      </c>
+      <c r="J26">
         <v>42</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1434,13 +1515,16 @@
         <v>6</v>
       </c>
       <c r="I27">
+        <v>67</v>
+      </c>
+      <c r="J27">
         <v>46</v>
       </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1466,13 +1550,16 @@
         <v>7</v>
       </c>
       <c r="I28">
+        <v>77</v>
+      </c>
+      <c r="J28">
         <v>50</v>
       </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -1498,13 +1585,16 @@
         <v>8</v>
       </c>
       <c r="I29">
+        <v>62</v>
+      </c>
+      <c r="J29">
         <v>49</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -1530,13 +1620,16 @@
         <v>9</v>
       </c>
       <c r="I30">
+        <v>95</v>
+      </c>
+      <c r="J30">
         <v>49</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -1562,13 +1655,16 @@
         <v>10</v>
       </c>
       <c r="I31">
+        <v>72</v>
+      </c>
+      <c r="J31">
         <v>46</v>
       </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -1594,13 +1690,16 @@
         <v>1</v>
       </c>
       <c r="I32">
+        <v>53</v>
+      </c>
+      <c r="J32">
         <v>51</v>
       </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1626,13 +1725,16 @@
         <v>2</v>
       </c>
       <c r="I33">
+        <v>78</v>
+      </c>
+      <c r="J33">
         <v>50</v>
       </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -1658,13 +1760,16 @@
         <v>3</v>
       </c>
       <c r="I34">
+        <v>59</v>
+      </c>
+      <c r="J34">
         <v>49</v>
       </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -1690,13 +1795,16 @@
         <v>4</v>
       </c>
       <c r="I35">
+        <v>36</v>
+      </c>
+      <c r="J35">
         <v>50</v>
       </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -1722,13 +1830,16 @@
         <v>5</v>
       </c>
       <c r="I36">
+        <v>73</v>
+      </c>
+      <c r="J36">
         <v>45</v>
       </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -1754,13 +1865,16 @@
         <v>6</v>
       </c>
       <c r="I37">
+        <v>67</v>
+      </c>
+      <c r="J37">
         <v>46</v>
       </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -1786,13 +1900,16 @@
         <v>7</v>
       </c>
       <c r="I38">
+        <v>77</v>
+      </c>
+      <c r="J38">
         <v>50</v>
       </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1818,13 +1935,16 @@
         <v>8</v>
       </c>
       <c r="I39">
+        <v>62</v>
+      </c>
+      <c r="J39">
         <v>50</v>
       </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>25</v>
       </c>
@@ -1850,13 +1970,16 @@
         <v>9</v>
       </c>
       <c r="I40">
+        <v>95</v>
+      </c>
+      <c r="J40">
         <v>48</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -1882,13 +2005,16 @@
         <v>10</v>
       </c>
       <c r="I41">
+        <v>72</v>
+      </c>
+      <c r="J41">
         <v>46</v>
       </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -1914,16 +2040,19 @@
         <v>1</v>
       </c>
       <c r="I42">
+        <v>53</v>
+      </c>
+      <c r="J42">
         <v>51</v>
       </c>
-      <c r="J42">
-        <v>0</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -1949,13 +2078,16 @@
         <v>2</v>
       </c>
       <c r="I43">
+        <v>78</v>
+      </c>
+      <c r="J43">
         <v>50</v>
       </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>25</v>
       </c>
@@ -1981,16 +2113,19 @@
         <v>3</v>
       </c>
       <c r="I44">
+        <v>59</v>
+      </c>
+      <c r="J44">
         <v>50</v>
       </c>
-      <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44" t="s">
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -2016,13 +2151,16 @@
         <v>4</v>
       </c>
       <c r="I45">
+        <v>36</v>
+      </c>
+      <c r="J45">
         <v>50</v>
       </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>25</v>
       </c>
@@ -2048,13 +2186,16 @@
         <v>5</v>
       </c>
       <c r="I46">
+        <v>73</v>
+      </c>
+      <c r="J46">
         <v>45</v>
       </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -2080,16 +2221,19 @@
         <v>6</v>
       </c>
       <c r="I47">
+        <v>67</v>
+      </c>
+      <c r="J47">
         <v>47</v>
       </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
-      <c r="K47" t="s">
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>25</v>
       </c>
@@ -2115,16 +2259,19 @@
         <v>7</v>
       </c>
       <c r="I48">
+        <v>77</v>
+      </c>
+      <c r="J48">
         <v>50</v>
       </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="K48" t="s">
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -2150,13 +2297,16 @@
         <v>8</v>
       </c>
       <c r="I49">
+        <v>62</v>
+      </c>
+      <c r="J49">
         <v>50</v>
       </c>
-      <c r="J49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -2182,13 +2332,16 @@
         <v>9</v>
       </c>
       <c r="I50">
+        <v>95</v>
+      </c>
+      <c r="J50">
         <v>48</v>
       </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>25</v>
       </c>
@@ -2214,13 +2367,16 @@
         <v>10</v>
       </c>
       <c r="I51">
+        <v>72</v>
+      </c>
+      <c r="J51">
         <v>46</v>
       </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>25</v>
       </c>
@@ -2246,13 +2402,16 @@
         <v>1</v>
       </c>
       <c r="I52">
+        <v>53</v>
+      </c>
+      <c r="J52">
         <v>51</v>
       </c>
-      <c r="J52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -2278,13 +2437,16 @@
         <v>2</v>
       </c>
       <c r="I53">
+        <v>78</v>
+      </c>
+      <c r="J53">
         <v>51</v>
       </c>
-      <c r="J53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>25</v>
       </c>
@@ -2310,13 +2472,16 @@
         <v>3</v>
       </c>
       <c r="I54">
+        <v>59</v>
+      </c>
+      <c r="J54">
         <v>50</v>
       </c>
-      <c r="J54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -2342,13 +2507,16 @@
         <v>4</v>
       </c>
       <c r="I55">
+        <v>36</v>
+      </c>
+      <c r="J55">
         <v>50</v>
       </c>
-      <c r="J55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -2374,16 +2542,19 @@
         <v>5</v>
       </c>
       <c r="I56">
+        <v>73</v>
+      </c>
+      <c r="J56">
         <v>43</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>1</v>
       </c>
-      <c r="K56" t="s">
+      <c r="L56" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>25</v>
       </c>
@@ -2409,13 +2580,16 @@
         <v>6</v>
       </c>
       <c r="I57">
+        <v>67</v>
+      </c>
+      <c r="J57">
         <v>47</v>
       </c>
-      <c r="J57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>25</v>
       </c>
@@ -2441,13 +2615,16 @@
         <v>7</v>
       </c>
       <c r="I58">
+        <v>77</v>
+      </c>
+      <c r="J58">
         <v>50</v>
       </c>
-      <c r="J58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>25</v>
       </c>
@@ -2473,13 +2650,16 @@
         <v>8</v>
       </c>
       <c r="I59">
+        <v>62</v>
+      </c>
+      <c r="J59">
         <v>50</v>
       </c>
-      <c r="J59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -2505,13 +2685,16 @@
         <v>9</v>
       </c>
       <c r="I60">
+        <v>95</v>
+      </c>
+      <c r="J60">
         <v>48</v>
       </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>25</v>
       </c>
@@ -2537,13 +2720,16 @@
         <v>10</v>
       </c>
       <c r="I61">
+        <v>72</v>
+      </c>
+      <c r="J61">
         <v>46</v>
       </c>
-      <c r="J61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>25</v>
       </c>
@@ -2569,13 +2755,16 @@
         <v>1</v>
       </c>
       <c r="I62">
+        <v>53</v>
+      </c>
+      <c r="J62">
         <v>51</v>
       </c>
-      <c r="J62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>25</v>
       </c>
@@ -2601,13 +2790,16 @@
         <v>2</v>
       </c>
       <c r="I63">
+        <v>78</v>
+      </c>
+      <c r="J63">
         <v>51</v>
       </c>
-      <c r="J63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>25</v>
       </c>
@@ -2633,13 +2825,16 @@
         <v>3</v>
       </c>
       <c r="I64">
+        <v>59</v>
+      </c>
+      <c r="J64">
         <v>50</v>
       </c>
-      <c r="J64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>25</v>
       </c>
@@ -2665,13 +2860,16 @@
         <v>4</v>
       </c>
       <c r="I65">
+        <v>36</v>
+      </c>
+      <c r="J65">
         <v>50</v>
       </c>
-      <c r="J65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -2697,13 +2895,16 @@
         <v>5</v>
       </c>
       <c r="I66">
+        <v>73</v>
+      </c>
+      <c r="J66">
         <v>43</v>
       </c>
-      <c r="J66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>25</v>
       </c>
@@ -2729,13 +2930,16 @@
         <v>6</v>
       </c>
       <c r="I67">
+        <v>67</v>
+      </c>
+      <c r="J67">
         <v>47</v>
       </c>
-      <c r="J67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>25</v>
       </c>
@@ -2761,13 +2965,16 @@
         <v>7</v>
       </c>
       <c r="I68">
+        <v>77</v>
+      </c>
+      <c r="J68">
         <v>50</v>
       </c>
-      <c r="J68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>25</v>
       </c>
@@ -2793,13 +3000,16 @@
         <v>8</v>
       </c>
       <c r="I69">
+        <v>62</v>
+      </c>
+      <c r="J69">
         <v>50</v>
       </c>
-      <c r="J69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>25</v>
       </c>
@@ -2825,13 +3035,16 @@
         <v>9</v>
       </c>
       <c r="I70">
+        <v>95</v>
+      </c>
+      <c r="J70">
         <v>48</v>
       </c>
-      <c r="J70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>25</v>
       </c>
@@ -2857,16 +3070,19 @@
         <v>10</v>
       </c>
       <c r="I71">
+        <v>72</v>
+      </c>
+      <c r="J71">
         <v>47</v>
       </c>
-      <c r="J71">
-        <v>0</v>
-      </c>
-      <c r="K71" t="s">
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>25</v>
       </c>
@@ -2892,13 +3108,16 @@
         <v>1</v>
       </c>
       <c r="I72">
+        <v>53</v>
+      </c>
+      <c r="J72">
         <v>51</v>
       </c>
-      <c r="J72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>25</v>
       </c>
@@ -2924,13 +3143,16 @@
         <v>2</v>
       </c>
       <c r="I73">
+        <v>78</v>
+      </c>
+      <c r="J73">
         <v>51</v>
       </c>
-      <c r="J73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>25</v>
       </c>
@@ -2956,13 +3178,16 @@
         <v>3</v>
       </c>
       <c r="I74">
+        <v>59</v>
+      </c>
+      <c r="J74">
         <v>50</v>
       </c>
-      <c r="J74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>25</v>
       </c>
@@ -2988,13 +3213,16 @@
         <v>4</v>
       </c>
       <c r="I75">
+        <v>36</v>
+      </c>
+      <c r="J75">
         <v>50</v>
       </c>
-      <c r="J75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>25</v>
       </c>
@@ -3020,13 +3248,16 @@
         <v>5</v>
       </c>
       <c r="I76">
+        <v>73</v>
+      </c>
+      <c r="J76">
         <v>43</v>
       </c>
-      <c r="J76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>25</v>
       </c>
@@ -3052,13 +3283,16 @@
         <v>6</v>
       </c>
       <c r="I77">
+        <v>67</v>
+      </c>
+      <c r="J77">
         <v>47</v>
       </c>
-      <c r="J77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>25</v>
       </c>
@@ -3084,13 +3318,16 @@
         <v>7</v>
       </c>
       <c r="I78">
+        <v>77</v>
+      </c>
+      <c r="J78">
         <v>50</v>
       </c>
-      <c r="J78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>25</v>
       </c>
@@ -3116,13 +3353,16 @@
         <v>8</v>
       </c>
       <c r="I79">
+        <v>62</v>
+      </c>
+      <c r="J79">
         <v>50</v>
       </c>
-      <c r="J79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>25</v>
       </c>
@@ -3148,13 +3388,16 @@
         <v>9</v>
       </c>
       <c r="I80">
+        <v>95</v>
+      </c>
+      <c r="J80">
         <v>48</v>
       </c>
-      <c r="J80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>25</v>
       </c>
@@ -3180,13 +3423,16 @@
         <v>10</v>
       </c>
       <c r="I81">
+        <v>72</v>
+      </c>
+      <c r="J81">
         <v>46</v>
       </c>
-      <c r="J81">
+      <c r="K81">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>25</v>
       </c>
@@ -3212,13 +3458,16 @@
         <v>1</v>
       </c>
       <c r="I82">
+        <v>53</v>
+      </c>
+      <c r="J82">
         <v>51</v>
       </c>
-      <c r="J82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>25</v>
       </c>
@@ -3244,13 +3493,16 @@
         <v>2</v>
       </c>
       <c r="I83">
+        <v>78</v>
+      </c>
+      <c r="J83">
         <v>51</v>
       </c>
-      <c r="J83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>25</v>
       </c>
@@ -3276,13 +3528,16 @@
         <v>3</v>
       </c>
       <c r="I84">
+        <v>59</v>
+      </c>
+      <c r="J84">
         <v>50</v>
       </c>
-      <c r="J84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>25</v>
       </c>
@@ -3308,13 +3563,16 @@
         <v>4</v>
       </c>
       <c r="I85">
+        <v>36</v>
+      </c>
+      <c r="J85">
         <v>51</v>
       </c>
-      <c r="J85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>25</v>
       </c>
@@ -3340,13 +3598,16 @@
         <v>5</v>
       </c>
       <c r="I86">
+        <v>73</v>
+      </c>
+      <c r="J86">
         <v>43</v>
       </c>
-      <c r="J86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>25</v>
       </c>
@@ -3372,13 +3633,16 @@
         <v>6</v>
       </c>
       <c r="I87">
+        <v>67</v>
+      </c>
+      <c r="J87">
         <v>47</v>
       </c>
-      <c r="J87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>25</v>
       </c>
@@ -3404,13 +3668,16 @@
         <v>7</v>
       </c>
       <c r="I88">
+        <v>77</v>
+      </c>
+      <c r="J88">
         <v>50</v>
       </c>
-      <c r="J88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>25</v>
       </c>
@@ -3436,13 +3703,16 @@
         <v>8</v>
       </c>
       <c r="I89">
+        <v>62</v>
+      </c>
+      <c r="J89">
         <v>50</v>
       </c>
-      <c r="J89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>25</v>
       </c>
@@ -3468,13 +3738,16 @@
         <v>9</v>
       </c>
       <c r="I90">
+        <v>95</v>
+      </c>
+      <c r="J90">
         <v>48</v>
       </c>
-      <c r="J90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>25</v>
       </c>
@@ -3500,16 +3773,19 @@
         <v>10</v>
       </c>
       <c r="I91">
+        <v>72</v>
+      </c>
+      <c r="J91">
         <v>45</v>
       </c>
-      <c r="J91">
-        <v>0</v>
-      </c>
-      <c r="K91" t="s">
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>25</v>
       </c>
@@ -3535,13 +3811,16 @@
         <v>1</v>
       </c>
       <c r="I92">
+        <v>53</v>
+      </c>
+      <c r="J92">
         <v>51</v>
       </c>
-      <c r="J92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>25</v>
       </c>
@@ -3567,13 +3846,16 @@
         <v>2</v>
       </c>
       <c r="I93">
+        <v>78</v>
+      </c>
+      <c r="J93">
         <v>51</v>
       </c>
-      <c r="J93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>25</v>
       </c>
@@ -3599,13 +3881,16 @@
         <v>3</v>
       </c>
       <c r="I94">
+        <v>59</v>
+      </c>
+      <c r="J94">
         <v>50</v>
       </c>
-      <c r="J94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>25</v>
       </c>
@@ -3631,16 +3916,19 @@
         <v>4</v>
       </c>
       <c r="I95">
+        <v>36</v>
+      </c>
+      <c r="J95">
         <v>51</v>
       </c>
-      <c r="J95">
-        <v>0</v>
-      </c>
-      <c r="K95" t="s">
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="L95" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>25</v>
       </c>
@@ -3666,13 +3954,16 @@
         <v>5</v>
       </c>
       <c r="I96">
+        <v>73</v>
+      </c>
+      <c r="J96">
         <v>43</v>
       </c>
-      <c r="J96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>25</v>
       </c>
@@ -3698,13 +3989,16 @@
         <v>6</v>
       </c>
       <c r="I97">
+        <v>67</v>
+      </c>
+      <c r="J97">
         <v>47</v>
       </c>
-      <c r="J97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>25</v>
       </c>
@@ -3730,13 +4024,16 @@
         <v>7</v>
       </c>
       <c r="I98">
+        <v>77</v>
+      </c>
+      <c r="J98">
         <v>50</v>
       </c>
-      <c r="J98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>25</v>
       </c>
@@ -3762,13 +4059,16 @@
         <v>8</v>
       </c>
       <c r="I99">
+        <v>62</v>
+      </c>
+      <c r="J99">
         <v>50</v>
       </c>
-      <c r="J99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>25</v>
       </c>
@@ -3794,13 +4094,16 @@
         <v>9</v>
       </c>
       <c r="I100">
+        <v>95</v>
+      </c>
+      <c r="J100">
         <v>48</v>
       </c>
-      <c r="J100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>25</v>
       </c>
@@ -3826,13 +4129,16 @@
         <v>10</v>
       </c>
       <c r="I101">
+        <v>72</v>
+      </c>
+      <c r="J101">
         <v>46</v>
       </c>
-      <c r="J101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>25</v>
       </c>
@@ -3858,13 +4164,16 @@
         <v>1</v>
       </c>
       <c r="I102">
+        <v>53</v>
+      </c>
+      <c r="J102">
         <v>51</v>
       </c>
-      <c r="J102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>25</v>
       </c>
@@ -3890,13 +4199,16 @@
         <v>2</v>
       </c>
       <c r="I103">
+        <v>78</v>
+      </c>
+      <c r="J103">
         <v>51</v>
       </c>
-      <c r="J103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>25</v>
       </c>
@@ -3922,16 +4234,19 @@
         <v>3</v>
       </c>
       <c r="I104">
+        <v>59</v>
+      </c>
+      <c r="J104">
         <v>51</v>
       </c>
-      <c r="J104">
-        <v>0</v>
-      </c>
-      <c r="K104" t="s">
+      <c r="K104">
+        <v>0</v>
+      </c>
+      <c r="L104" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>25</v>
       </c>
@@ -3957,13 +4272,16 @@
         <v>4</v>
       </c>
       <c r="I105">
+        <v>36</v>
+      </c>
+      <c r="J105">
         <v>51</v>
       </c>
-      <c r="J105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>25</v>
       </c>
@@ -3989,13 +4307,16 @@
         <v>5</v>
       </c>
       <c r="I106">
+        <v>73</v>
+      </c>
+      <c r="J106">
         <v>43</v>
       </c>
-      <c r="J106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>25</v>
       </c>
@@ -4021,13 +4342,16 @@
         <v>6</v>
       </c>
       <c r="I107">
+        <v>67</v>
+      </c>
+      <c r="J107">
         <v>47</v>
       </c>
-      <c r="J107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>25</v>
       </c>
@@ -4053,13 +4377,16 @@
         <v>7</v>
       </c>
       <c r="I108">
+        <v>77</v>
+      </c>
+      <c r="J108">
         <v>50</v>
       </c>
-      <c r="J108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>25</v>
       </c>
@@ -4085,13 +4412,16 @@
         <v>8</v>
       </c>
       <c r="I109">
+        <v>62</v>
+      </c>
+      <c r="J109">
         <v>50</v>
       </c>
-      <c r="J109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>25</v>
       </c>
@@ -4117,13 +4447,16 @@
         <v>9</v>
       </c>
       <c r="I110">
+        <v>95</v>
+      </c>
+      <c r="J110">
         <v>48</v>
       </c>
-      <c r="J110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>25</v>
       </c>
@@ -4149,13 +4482,16 @@
         <v>10</v>
       </c>
       <c r="I111">
+        <v>72</v>
+      </c>
+      <c r="J111">
         <v>46</v>
       </c>
-      <c r="J111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>25</v>
       </c>
@@ -4181,16 +4517,19 @@
         <v>1</v>
       </c>
       <c r="I112">
+        <v>53</v>
+      </c>
+      <c r="J112">
         <v>50</v>
       </c>
-      <c r="J112">
-        <v>0</v>
-      </c>
-      <c r="K112" t="s">
+      <c r="K112">
+        <v>0</v>
+      </c>
+      <c r="L112" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>25</v>
       </c>
@@ -4216,13 +4555,16 @@
         <v>2</v>
       </c>
       <c r="I113">
+        <v>78</v>
+      </c>
+      <c r="J113">
         <v>51</v>
       </c>
-      <c r="J113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>25</v>
       </c>
@@ -4248,16 +4590,19 @@
         <v>3</v>
       </c>
       <c r="I114">
+        <v>59</v>
+      </c>
+      <c r="J114">
         <v>50</v>
       </c>
-      <c r="J114">
-        <v>0</v>
-      </c>
-      <c r="K114" t="s">
+      <c r="K114">
+        <v>0</v>
+      </c>
+      <c r="L114" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>25</v>
       </c>
@@ -4283,13 +4628,16 @@
         <v>4</v>
       </c>
       <c r="I115">
+        <v>36</v>
+      </c>
+      <c r="J115">
         <v>51</v>
       </c>
-      <c r="J115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>25</v>
       </c>
@@ -4315,13 +4663,16 @@
         <v>5</v>
       </c>
       <c r="I116">
+        <v>73</v>
+      </c>
+      <c r="J116">
         <v>43</v>
       </c>
-      <c r="J116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>25</v>
       </c>
@@ -4347,13 +4698,16 @@
         <v>6</v>
       </c>
       <c r="I117">
+        <v>67</v>
+      </c>
+      <c r="J117">
         <v>47</v>
       </c>
-      <c r="J117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>25</v>
       </c>
@@ -4379,13 +4733,16 @@
         <v>7</v>
       </c>
       <c r="I118">
+        <v>77</v>
+      </c>
+      <c r="J118">
         <v>50</v>
       </c>
-      <c r="J118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>25</v>
       </c>
@@ -4411,13 +4768,16 @@
         <v>8</v>
       </c>
       <c r="I119">
+        <v>62</v>
+      </c>
+      <c r="J119">
         <v>50</v>
       </c>
-      <c r="J119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>25</v>
       </c>
@@ -4443,13 +4803,16 @@
         <v>9</v>
       </c>
       <c r="I120">
+        <v>95</v>
+      </c>
+      <c r="J120">
         <v>48</v>
       </c>
-      <c r="J120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>25</v>
       </c>
@@ -4475,13 +4838,16 @@
         <v>10</v>
       </c>
       <c r="I121">
+        <v>72</v>
+      </c>
+      <c r="J121">
         <v>46</v>
       </c>
-      <c r="J121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>25</v>
       </c>
@@ -4507,16 +4873,19 @@
         <v>1</v>
       </c>
       <c r="I122">
+        <v>53</v>
+      </c>
+      <c r="J122">
         <v>48</v>
       </c>
-      <c r="J122">
+      <c r="K122">
         <v>2</v>
       </c>
-      <c r="K122" t="s">
+      <c r="L122" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>25</v>
       </c>
@@ -4542,13 +4911,16 @@
         <v>2</v>
       </c>
       <c r="I123">
+        <v>78</v>
+      </c>
+      <c r="J123">
         <v>51</v>
       </c>
-      <c r="J123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>25</v>
       </c>
@@ -4574,13 +4946,16 @@
         <v>3</v>
       </c>
       <c r="I124">
+        <v>59</v>
+      </c>
+      <c r="J124">
         <v>49</v>
       </c>
-      <c r="J124">
+      <c r="K124">
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>25</v>
       </c>
@@ -4606,13 +4981,16 @@
         <v>4</v>
       </c>
       <c r="I125">
+        <v>36</v>
+      </c>
+      <c r="J125">
         <v>51</v>
       </c>
-      <c r="J125">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>25</v>
       </c>
@@ -4638,13 +5016,16 @@
         <v>5</v>
       </c>
       <c r="I126">
+        <v>73</v>
+      </c>
+      <c r="J126">
         <v>43</v>
       </c>
-      <c r="J126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>25</v>
       </c>
@@ -4670,13 +5051,16 @@
         <v>6</v>
       </c>
       <c r="I127">
+        <v>67</v>
+      </c>
+      <c r="J127">
         <v>47</v>
       </c>
-      <c r="J127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>25</v>
       </c>
@@ -4702,13 +5086,16 @@
         <v>7</v>
       </c>
       <c r="I128">
+        <v>77</v>
+      </c>
+      <c r="J128">
         <v>50</v>
       </c>
-      <c r="J128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>25</v>
       </c>
@@ -4734,13 +5121,16 @@
         <v>8</v>
       </c>
       <c r="I129">
+        <v>62</v>
+      </c>
+      <c r="J129">
         <v>50</v>
       </c>
-      <c r="J129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>25</v>
       </c>
@@ -4766,13 +5156,16 @@
         <v>9</v>
       </c>
       <c r="I130">
+        <v>95</v>
+      </c>
+      <c r="J130">
         <v>48</v>
       </c>
-      <c r="J130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>25</v>
       </c>
@@ -4798,9 +5191,12 @@
         <v>10</v>
       </c>
       <c r="I131">
+        <v>72</v>
+      </c>
+      <c r="J131">
         <v>46</v>
       </c>
-      <c r="J131">
+      <c r="K131">
         <v>0</v>
       </c>
     </row>

</xml_diff>